<commit_message>
all the necessary stuff finished
</commit_message>
<xml_diff>
--- a/Info/Workbook1.xlsx
+++ b/Info/Workbook1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yaroslava/Google Drive/Study | ALL (current)/IASA | System Analysis/SA-lab5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Yaroslava/Google Drive/Study | ALL (current)/IASA | System Analysis/SA-lab5/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="460" windowWidth="24220" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,23 +27,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="80">
   <si>
     <t>Корпус</t>
   </si>
   <si>
-    <t>Вес(г)</t>
-  </si>
-  <si>
-    <t>портативность</t>
-  </si>
-  <si>
     <t xml:space="preserve">Материал </t>
   </si>
   <si>
-    <t>цена</t>
-  </si>
-  <si>
     <t>AgDrone</t>
   </si>
   <si>
@@ -71,9 +62,6 @@
     <t>Двигуни</t>
   </si>
   <si>
-    <t>Двигун</t>
-  </si>
-  <si>
     <t>Вес</t>
   </si>
   <si>
@@ -119,9 +107,6 @@
     <t>Пропелери</t>
   </si>
   <si>
-    <t>Пропелер</t>
-  </si>
-  <si>
     <t>Материал</t>
   </si>
   <si>
@@ -179,9 +164,6 @@
     <t>Кількість ядер</t>
   </si>
   <si>
-    <t>Ціна</t>
-  </si>
-  <si>
     <t>Частота</t>
   </si>
   <si>
@@ -279,6 +261,12 @@
   </si>
   <si>
     <t xml:space="preserve">WL Toys WLFalseQ282Jw </t>
+  </si>
+  <si>
+    <t>Название</t>
+  </si>
+  <si>
+    <t>Портативность</t>
   </si>
 </sst>
 </file>
@@ -367,7 +355,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -481,12 +469,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -510,9 +548,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -535,29 +570,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -578,9 +598,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,44 +609,119 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -911,554 +1003,541 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53:F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="16.6640625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="26" style="19" customWidth="1"/>
-    <col min="4" max="4" width="20" style="19" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="19" customWidth="1"/>
-    <col min="6" max="6" width="18.33203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="18" style="19" customWidth="1"/>
+    <col min="2" max="3" width="16.6640625" style="17" customWidth="1"/>
+    <col min="4" max="4" width="20" style="17" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="18" style="17" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" style="3" customWidth="1"/>
     <col min="9" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="34" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
+    <row r="1" spans="2:10" s="27" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="59" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="26"/>
     </row>
     <row r="2" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="7"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
     </row>
     <row r="3" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="28" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="29" t="s">
+      <c r="B3" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11">
+    <row r="4" spans="2:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="B4" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="13">
+        <v>15000</v>
+      </c>
+      <c r="D4" s="14">
         <v>180</v>
       </c>
-      <c r="D4" s="11" t="b">
+      <c r="E4" s="13" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="12">
-        <v>15000</v>
-      </c>
-      <c r="G4" s="13"/>
-      <c r="H4" s="6"/>
+      <c r="F4" s="14" t="s">
+        <v>3</v>
+      </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
     <row r="5" spans="2:10" ht="47" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="14">
+      <c r="B5" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <v>10500</v>
+      </c>
+      <c r="D5" s="38">
         <v>230</v>
       </c>
-      <c r="D5" s="14" t="b">
+      <c r="E5" s="39" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="15">
-        <v>10500</v>
-      </c>
-      <c r="G5" s="13"/>
-      <c r="H5" s="6"/>
+      <c r="F5" s="38" t="s">
+        <v>5</v>
+      </c>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="8"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="6"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="38"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" s="11">
+      <c r="B7" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="13">
+        <v>7000</v>
+      </c>
+      <c r="D7" s="14">
         <v>300</v>
       </c>
-      <c r="D7" s="11" t="b">
+      <c r="E7" s="13" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="12">
-        <v>7000</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="6"/>
+      <c r="F7" s="14" t="s">
+        <v>7</v>
+      </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="11">
+    <row r="8" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="20">
+        <v>8000</v>
+      </c>
+      <c r="D8" s="19">
         <v>450</v>
       </c>
-      <c r="D8" s="11" t="b">
+      <c r="E8" s="20" t="b">
         <v>0</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="12">
-        <v>8000</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="6"/>
+      <c r="F8" s="19" t="s">
+        <v>9</v>
+      </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
     </row>
-    <row r="9" spans="2:10" s="34" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="C9" s="38"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="38"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
+    <row r="9" spans="2:10" s="27" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="29"/>
+      <c r="J9" s="29"/>
     </row>
     <row r="10" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="B10" s="52" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="37"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="28" t="s">
+      <c r="B11" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="29" t="s">
+      <c r="G11" s="24" t="s">
         <v>15</v>
-      </c>
-      <c r="E11" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>19</v>
       </c>
       <c r="H11" s="6"/>
       <c r="J11" s="6"/>
     </row>
     <row r="12" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B12" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="11">
+      <c r="B12" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="32">
         <v>10000</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="33">
         <v>160</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="F12" s="11">
+      <c r="E12" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="10">
         <v>6</v>
       </c>
-      <c r="G12" s="12" t="s">
-        <v>22</v>
+      <c r="G12" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="H12" s="6"/>
       <c r="J12" s="6"/>
     </row>
     <row r="13" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="11">
+      <c r="B13" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="13">
         <v>8000</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="14">
         <v>200</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F13" s="11">
+      <c r="E13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="10">
         <v>4</v>
       </c>
-      <c r="G13" s="12" t="s">
-        <v>22</v>
+      <c r="G13" s="11" t="s">
+        <v>18</v>
       </c>
       <c r="H13" s="6"/>
       <c r="J13" s="6"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C14" s="11">
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="13">
         <v>5000</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="14">
         <v>320</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="E14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="10">
         <v>4</v>
       </c>
-      <c r="G14" s="12" t="s">
-        <v>26</v>
+      <c r="G14" s="11" t="s">
+        <v>22</v>
       </c>
       <c r="H14" s="6"/>
       <c r="J14" s="6"/>
     </row>
     <row r="15" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" s="17">
+      <c r="B15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="20">
         <v>1000</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="19">
         <v>130</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="17">
+      <c r="E15" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="16">
         <v>2</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="H15" s="6"/>
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="22"/>
+      <c r="B16" s="55" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="54"/>
+      <c r="D16" s="54"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37"/>
       <c r="G16" s="7"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="G17" s="13"/>
+      <c r="B17" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="12"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B18" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="11">
+      <c r="B18" s="53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="32">
         <v>200</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="33">
         <v>30</v>
       </c>
-      <c r="E18" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="12">
+      <c r="E18" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="11">
         <v>2</v>
       </c>
-      <c r="G18" s="13"/>
+      <c r="G18" s="12"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B19" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C19" s="11">
+      <c r="B19" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="13">
         <v>150</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="14">
         <v>50</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F19" s="12">
+      <c r="E19" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="11">
         <v>2</v>
       </c>
-      <c r="G19" s="13"/>
+      <c r="G19" s="12"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B20" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="14">
+      <c r="B20" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" s="39">
         <v>240</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="38">
         <v>130</v>
       </c>
-      <c r="E20" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="F20" s="15">
+      <c r="E20" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="38">
         <v>6</v>
       </c>
-      <c r="G20" s="13"/>
+      <c r="G20" s="12"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B21" s="18"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="13"/>
+      <c r="B21" s="41"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="39"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="12"/>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
     </row>
     <row r="22" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="17">
+      <c r="B22" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="20">
         <v>245</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="19">
         <v>75</v>
       </c>
-      <c r="E22" s="17" t="s">
-        <v>35</v>
+      <c r="E22" s="16" t="s">
+        <v>30</v>
       </c>
       <c r="F22" s="1">
         <v>4</v>
       </c>
-      <c r="G22" s="13"/>
+      <c r="G22" s="12"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
     </row>
-    <row r="23" spans="2:10" s="34" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="41"/>
-      <c r="G23" s="35"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+    <row r="23" spans="2:10" s="27" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="62" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="63"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
     </row>
     <row r="24" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="C24" s="21"/>
-      <c r="D24" s="21"/>
-      <c r="E24" s="21"/>
-      <c r="F24" s="22"/>
+      <c r="B24" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="37"/>
       <c r="G24" s="7"/>
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="45" t="s">
-        <v>82</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>40</v>
+      <c r="B25" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>35</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6"/>
       <c r="J25" s="6"/>
     </row>
     <row r="26" spans="2:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="B26" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="12">
+      <c r="B26" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="11">
         <v>750</v>
       </c>
-      <c r="D26" s="10" t="b">
+      <c r="D26" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="E26" s="11" t="b">
+      <c r="E26" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F26" s="46" t="s">
-        <v>42</v>
+      <c r="F26" s="31" t="s">
+        <v>37</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6"/>
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B27" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C27" s="12">
+      <c r="B27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C27" s="11">
         <v>640</v>
       </c>
-      <c r="D27" s="10" t="b">
+      <c r="D27" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="E27" s="11" t="b">
+      <c r="E27" s="10" t="b">
         <v>1</v>
       </c>
-      <c r="F27" s="46" t="s">
-        <v>44</v>
+      <c r="F27" s="31" t="s">
+        <v>39</v>
       </c>
       <c r="H27" s="6"/>
       <c r="I27" s="6"/>
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B28" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="12">
+      <c r="B28" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="11">
         <v>360</v>
       </c>
-      <c r="D28" s="10" t="b">
+      <c r="D28" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="E28" s="11" t="b">
+      <c r="E28" s="10" t="b">
         <v>0</v>
       </c>
-      <c r="F28" s="46" t="s">
-        <v>46</v>
+      <c r="F28" s="31" t="s">
+        <v>41</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6"/>
       <c r="J28" s="6"/>
     </row>
     <row r="29" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="16" t="s">
-        <v>47</v>
+      <c r="B29" s="15" t="s">
+        <v>42</v>
       </c>
       <c r="C29" s="1">
         <v>260</v>
       </c>
-      <c r="D29" s="23" t="b">
+      <c r="D29" s="18" t="b">
         <v>0</v>
       </c>
-      <c r="E29" s="17" t="b">
+      <c r="E29" s="16" t="b">
         <v>0</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="6"/>
       <c r="J29" s="6"/>
     </row>
     <row r="30" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="22"/>
+      <c r="B30" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="36"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="49"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1466,100 +1545,100 @@
       <c r="J30" s="5"/>
     </row>
     <row r="31" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="C31" s="29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="11"/>
+      <c r="B31" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="E31" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G31" s="10"/>
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B32" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C32" s="11">
+      <c r="B32" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="C32" s="13">
         <v>460</v>
       </c>
-      <c r="D32" s="12">
+      <c r="D32" s="34">
         <v>1.8</v>
       </c>
-      <c r="E32" s="12">
+      <c r="E32" s="14">
         <v>6</v>
       </c>
-      <c r="G32" s="11"/>
+      <c r="G32" s="10"/>
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B33" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="11">
+      <c r="B33" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="13">
         <v>980</v>
       </c>
-      <c r="D33" s="12">
+      <c r="D33" s="34">
         <v>2.7</v>
       </c>
-      <c r="E33" s="12">
+      <c r="E33" s="14">
         <v>8</v>
       </c>
-      <c r="G33" s="11"/>
+      <c r="G33" s="10"/>
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B34" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="C34" s="11">
+      <c r="B34" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="13">
         <v>145</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="34">
         <v>1.6</v>
       </c>
-      <c r="E34" s="12">
+      <c r="E34" s="14">
         <v>4</v>
       </c>
-      <c r="G34" s="11"/>
+      <c r="G34" s="10"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
     </row>
     <row r="35" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="C35" s="17">
+      <c r="B35" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="20">
         <v>750</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="18">
         <v>3</v>
       </c>
-      <c r="E35" s="1">
+      <c r="E35" s="19">
         <v>8</v>
       </c>
-      <c r="G35" s="11"/>
+      <c r="G35" s="10"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
     </row>
     <row r="36" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="22"/>
+      <c r="B36" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" s="37"/>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
@@ -1568,12 +1647,12 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
     </row>
-    <row r="37" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="31" t="s">
-        <v>57</v>
+    <row r="37" spans="2:10" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>51</v>
       </c>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
@@ -1584,10 +1663,10 @@
       <c r="J37" s="6"/>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B38" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C38" s="15">
+      <c r="B38" s="57" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="38">
         <v>1</v>
       </c>
       <c r="D38" s="6"/>
@@ -1599,8 +1678,8 @@
       <c r="J38" s="6"/>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B39" s="18"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="57"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
@@ -1610,10 +1689,10 @@
       <c r="J39" s="6"/>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B40" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="C40" s="12">
+      <c r="B40" s="51" t="s">
+        <v>53</v>
+      </c>
+      <c r="C40" s="11">
         <v>2</v>
       </c>
       <c r="D40" s="6"/>
@@ -1625,10 +1704,10 @@
       <c r="J40" s="6"/>
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B41" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="12">
+      <c r="B41" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="C41" s="11">
         <v>3</v>
       </c>
       <c r="D41" s="6"/>
@@ -1640,10 +1719,10 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B42" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="15">
+      <c r="B42" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="C42" s="38">
         <v>0.5</v>
       </c>
       <c r="D42" s="6"/>
@@ -1655,8 +1734,8 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="18"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="38"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
@@ -1666,200 +1745,200 @@
       <c r="J43" s="6"/>
     </row>
     <row r="44" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C44" s="21"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="21"/>
-      <c r="F44" s="22"/>
+      <c r="B44" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="37"/>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
     </row>
     <row r="45" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="C45" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D45" s="29" t="s">
-        <v>63</v>
-      </c>
-      <c r="E45" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="F45" s="31" t="s">
-        <v>65</v>
+      <c r="B45" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C45" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E45" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="25" t="s">
+        <v>59</v>
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6"/>
     </row>
     <row r="46" spans="2:10" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="C46" s="47">
+      <c r="B46" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C46" s="42">
         <v>1750</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="39">
         <v>2.4</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="39">
         <v>180</v>
       </c>
-      <c r="F46" s="48">
+      <c r="F46" s="42">
         <v>35</v>
       </c>
       <c r="I46" s="6"/>
       <c r="J46" s="6"/>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B47" s="18"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="15"/>
+      <c r="B47" s="41"/>
+      <c r="C47" s="38"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="38"/>
       <c r="I47" s="6"/>
       <c r="J47" s="6"/>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B48" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="C48" s="14">
+      <c r="B48" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="38">
         <v>1200</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="39">
         <v>2</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="39">
         <v>180</v>
       </c>
-      <c r="F48" s="15">
+      <c r="F48" s="38">
         <v>18</v>
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="6"/>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B49" s="18"/>
-      <c r="C49" s="14"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="14"/>
-      <c r="F49" s="15"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="38"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="38"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B50" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="11">
+      <c r="B50" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="C50" s="14">
         <v>980</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="10">
         <v>2.4</v>
       </c>
-      <c r="E50" s="11">
+      <c r="E50" s="10">
         <v>105</v>
       </c>
-      <c r="F50" s="12">
+      <c r="F50" s="11">
         <v>15</v>
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6"/>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B51" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="C51" s="14">
+      <c r="B51" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="38">
         <v>330</v>
       </c>
-      <c r="D51" s="14">
+      <c r="D51" s="39">
         <v>1.5</v>
       </c>
-      <c r="E51" s="14">
+      <c r="E51" s="39">
         <v>90</v>
       </c>
-      <c r="F51" s="15">
+      <c r="F51" s="38">
         <v>10</v>
       </c>
       <c r="I51" s="6"/>
       <c r="J51" s="6"/>
     </row>
     <row r="52" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="24"/>
-      <c r="C52" s="26"/>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="25"/>
+      <c r="B52" s="45"/>
+      <c r="C52" s="43"/>
+      <c r="D52" s="44"/>
+      <c r="E52" s="44"/>
+      <c r="F52" s="43"/>
       <c r="I52" s="6"/>
       <c r="J52" s="6"/>
     </row>
-    <row r="53" spans="2:10" s="34" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="C53" s="43"/>
-      <c r="D53" s="43"/>
-      <c r="E53" s="43"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="36"/>
-      <c r="H53" s="36"/>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
+    <row r="53" spans="2:10" s="27" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C53" s="66"/>
+      <c r="D53" s="66"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="67"/>
+      <c r="G53" s="29"/>
+      <c r="H53" s="29"/>
+      <c r="I53" s="29"/>
+      <c r="J53" s="29"/>
     </row>
     <row r="54" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="C54" s="21"/>
-      <c r="D54" s="21"/>
-      <c r="E54" s="21"/>
-      <c r="F54" s="22"/>
+      <c r="B54" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="36"/>
+      <c r="F54" s="37"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
     </row>
     <row r="55" spans="2:10" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="C55" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D55" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="E55" s="29" t="s">
-        <v>72</v>
-      </c>
-      <c r="F55" s="31" t="s">
-        <v>73</v>
+      <c r="B55" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C55" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="E55" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="F55" s="25" t="s">
+        <v>67</v>
       </c>
       <c r="H55" s="6"/>
       <c r="I55" s="6"/>
       <c r="J55" s="6"/>
     </row>
     <row r="56" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B56" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="C56" s="15">
+      <c r="B56" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="C56" s="38">
         <v>1400</v>
       </c>
-      <c r="D56" s="49">
+      <c r="D56" s="46">
         <v>360</v>
       </c>
-      <c r="E56" s="11">
+      <c r="E56" s="10">
         <v>5</v>
       </c>
-      <c r="F56" s="12">
+      <c r="F56" s="11">
         <v>150</v>
       </c>
       <c r="H56" s="6"/>
@@ -1867,29 +1946,29 @@
       <c r="J56" s="6"/>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B57" s="18"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="49"/>
-      <c r="E57" s="11"/>
-      <c r="F57" s="12"/>
+      <c r="B57" s="41"/>
+      <c r="C57" s="38"/>
+      <c r="D57" s="46"/>
+      <c r="E57" s="10"/>
+      <c r="F57" s="11"/>
       <c r="H57" s="6"/>
       <c r="I57" s="6"/>
       <c r="J57" s="6"/>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B58" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="12">
+      <c r="B58" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="C58" s="11">
         <v>800</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D58" s="9">
         <v>60</v>
       </c>
-      <c r="E58" s="11">
+      <c r="E58" s="10">
         <v>4</v>
       </c>
-      <c r="F58" s="12">
+      <c r="F58" s="11">
         <v>300</v>
       </c>
       <c r="H58" s="6"/>
@@ -1897,19 +1976,19 @@
       <c r="J58" s="6"/>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B59" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="12">
+      <c r="B59" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C59" s="11">
         <v>600</v>
       </c>
-      <c r="D59" s="10">
+      <c r="D59" s="9">
         <v>120</v>
       </c>
-      <c r="E59" s="11">
+      <c r="E59" s="10">
         <v>10</v>
       </c>
-      <c r="F59" s="12">
+      <c r="F59" s="11">
         <v>400</v>
       </c>
       <c r="H59" s="6"/>
@@ -1917,16 +1996,16 @@
       <c r="J59" s="6"/>
     </row>
     <row r="60" spans="2:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B60" s="23" t="s">
-        <v>77</v>
+      <c r="B60" s="18" t="s">
+        <v>71</v>
       </c>
       <c r="C60" s="1">
         <v>2100</v>
       </c>
-      <c r="D60" s="23">
+      <c r="D60" s="18">
         <v>240</v>
       </c>
-      <c r="E60" s="17">
+      <c r="E60" s="16">
         <v>8</v>
       </c>
       <c r="F60" s="1">
@@ -1937,28 +2016,17 @@
       <c r="J60" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="44">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B9:G9"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B30:E30"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B36:C36"/>
+  <mergeCells count="43">
+    <mergeCell ref="B54:F54"/>
+    <mergeCell ref="B53:F53"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="D56:D57"/>
+    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="B51:B52"/>
     <mergeCell ref="C42:C43"/>
     <mergeCell ref="B42:B43"/>
     <mergeCell ref="B44:F44"/>
@@ -1972,16 +2040,26 @@
     <mergeCell ref="C48:C49"/>
     <mergeCell ref="E48:E49"/>
     <mergeCell ref="D48:D49"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="B54:F54"/>
-    <mergeCell ref="B53:F53"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="D56:D57"/>
-    <mergeCell ref="B56:B57"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B30:E30"/>
+    <mergeCell ref="C38:C39"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B5" r:id="rId1" tooltip="Hubsan H501S X4 (RTF, FPV)"/>

</xml_diff>